<commit_message>
bash files set up
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,35 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Qeetoto-Scripts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDDDEEA-51D5-BC49-9900-6C2EA6911D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17540" windowWidth="28800" xWindow="0" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Provider Name</t>
+  </si>
+  <si>
+    <t>Game Name</t>
+  </si>
+  <si>
+    <t>Number Of Plays</t>
+  </si>
+  <si>
+    <t>Difference To Mean</t>
+  </si>
+  <si>
+    <t>Average Stake</t>
+  </si>
+  <si>
+    <t>Unique Players</t>
+  </si>
+  <si>
+    <t>Turnover</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Operator Name/Date</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,16 +86,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -342,199 +392,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="13.6640625"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Operator Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Provider Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Game Name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Number Of Plays</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Difference To Mean</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Average Stake</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Unique Players</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Turnover</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Margin</t>
-        </is>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>43934</v>
-      </c>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>William Hill Riga</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Qeetoto</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Texas HedgeEm</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.5</v>
-      </c>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.5</v>
-      </c>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>43934</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>William Hill Riga</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Qeetoto</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Texas HedgeEm</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>100</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.5</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>